<commit_message>
Backup QR Scanner data - 20/05/2025, 2:26:18 PM
</commit_message>
<xml_diff>
--- a/backups/Scanner_Pharmacology_2025-05-20T10-18-14.xlsx
+++ b/backups/Scanner_Pharmacology_2025-05-20T10-18-14.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Pharmacology" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -430,7 +430,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C2" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D2" t="str">
         <v>13:18:22</v>
@@ -450,7 +450,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C3" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D3" t="str">
         <v>13:19:13</v>
@@ -470,7 +470,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C4" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D4" t="str">
         <v>13:20:00</v>
@@ -490,7 +490,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C5" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D5" t="str">
         <v>13:20:11</v>
@@ -510,7 +510,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C6" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D6" t="str">
         <v>13:26:16</v>
@@ -530,7 +530,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C7" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D7" t="str">
         <v>13:26:22</v>
@@ -550,7 +550,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C8" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D8" t="str">
         <v>13:45:23</v>
@@ -570,7 +570,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C9" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D9" t="str">
         <v>13:45:43</v>
@@ -590,7 +590,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C10" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D10" t="str">
         <v>13:45:50</v>
@@ -610,7 +610,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C11" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D11" t="str">
         <v>13:45:56</v>
@@ -630,7 +630,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C12" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D12" t="str">
         <v>13:46:07</v>
@@ -650,7 +650,7 @@
         <v>Pharmacology</v>
       </c>
       <c r="C13" t="str">
-        <v>05/20/2025</v>
+        <v>20/05/2025</v>
       </c>
       <c r="D13" t="str">
         <v>13:46:59</v>

</xml_diff>